<commit_message>
add favicon, add separator, add content for sections
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="-20" windowWidth="25040" windowHeight="17520" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="320" yWindow="0" windowWidth="25040" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="105">
   <si>
     <t>Anthony</t>
   </si>
@@ -498,6 +499,45 @@
 end to end process from workshop to research to design
 marketing and branding (patternlab, brand guidelines) 
 front-end (MVW, Js)</t>
+  </si>
+  <si>
+    <t>Juin 2015</t>
+  </si>
+  <si>
+    <t>Juillet 2015</t>
+  </si>
+  <si>
+    <t>Aout 2015</t>
+  </si>
+  <si>
+    <t>Septembre 2015</t>
+  </si>
+  <si>
+    <t>Octobre 2015</t>
+  </si>
+  <si>
+    <t>Novembre 2015</t>
+  </si>
+  <si>
+    <t>Decembre 2015</t>
+  </si>
+  <si>
+    <t>Janvier 2016</t>
+  </si>
+  <si>
+    <t>Fevrier 2016</t>
+  </si>
+  <si>
+    <t>Mars 2016</t>
+  </si>
+  <si>
+    <t>Avril 2016</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>http://www.creativebloq.com/ux/product-portfolios-61412126</t>
   </si>
 </sst>
 </file>
@@ -574,8 +614,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -594,13 +646,25 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1087,102 +1151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>5576430</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1226,6 +1198,9 @@
       <c r="D2" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="F2" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="75">
       <c r="A3" t="s">
@@ -1356,12 +1331,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1584,4 +1559,217 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>5576430</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13">
+        <f>SUM(B1:B11)</f>
+        <v>1958</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix nav bug on mobile view, change style and layout for work section, fix grid system layout
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="0" windowWidth="25040" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="420" yWindow="0" windowWidth="25040" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -614,8 +614,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -646,7 +650,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -656,6 +660,8 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -665,6 +671,8 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1153,7 +1161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -1658,7 +1666,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B11"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>